<commit_message>
adds pdf version of risk managemente
</commit_message>
<xml_diff>
--- a/doc/risks/Risk Management.xlsx
+++ b/doc/risks/Risk Management.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptrey\Documents\Software Engineering\vnvDoc\doc\risks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\bwSyncAndShare\vnvDoc\doc\risks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -167,6 +167,9 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <family val="2"/>
@@ -181,9 +184,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,13 +201,16 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F10" totalsRowShown="0">
   <autoFilter ref="A1:F10"/>
+  <sortState ref="A2:F10">
+    <sortCondition descending="1" ref="F1:F10"/>
+  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Identified" dataDxfId="0"/>
+    <tableColumn id="1" name="Identified" dataDxfId="1"/>
     <tableColumn id="2" name="prob of occurrence"/>
     <tableColumn id="3" name="damage"/>
     <tableColumn id="4" name="mitigation strategy"/>
     <tableColumn id="5" name="person in charge"/>
-    <tableColumn id="6" name="Risk factor" dataDxfId="1">
+    <tableColumn id="6" name="Risk factor" dataDxfId="0">
       <calculatedColumnFormula>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -570,65 +573,65 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.06</v>
+        <v>0.21000000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,44 +657,44 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -717,28 +720,28 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10">
         <f>Tabelle1[[#This Row],[prob of occurrence]]*Tabelle1[[#This Row],[damage]]</f>
-        <v>0.21000000000000002</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>